<commit_message>
method call and references
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7725"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7725" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="references-latest" sheetId="28" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4229" uniqueCount="2476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="2510">
   <si>
     <t>USER</t>
   </si>
@@ -7652,6 +7652,108 @@
   </si>
   <si>
     <t>sysout(p2.weight)</t>
+  </si>
+  <si>
+    <t>MethodTest.main : 7</t>
+  </si>
+  <si>
+    <t>Encounter return statement</t>
+  </si>
+  <si>
+    <t>or end of your method</t>
+  </si>
+  <si>
+    <t>METHOD STACK Memory</t>
+  </si>
+  <si>
+    <t>Methods.m3 : 17</t>
+  </si>
+  <si>
+    <t>Methods.m1: 5</t>
+  </si>
+  <si>
+    <t>Methods.m2 : 12</t>
+  </si>
+  <si>
+    <t>public class Methods {</t>
+  </si>
+  <si>
+    <t>public void test(int a,Person p) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         System.out.println(a);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         System.out.println(p.name);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         p.name="jane";</t>
+  </si>
+  <si>
+    <t>System.out.println("main");</t>
+  </si>
+  <si>
+    <t>Methods m=new Methods();</t>
+  </si>
+  <si>
+    <t>m.test(x, p1);</t>
+  </si>
+  <si>
+    <t>System.out.println(x);</t>
+  </si>
+  <si>
+    <t>System.out.println(p1.name);</t>
+  </si>
+  <si>
+    <t>PSVM</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>PRINTS</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>Method Stack</t>
+  </si>
+  <si>
+    <t>main:204</t>
+  </si>
+  <si>
+    <t>Pass By value</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>Pass by reference</t>
+  </si>
+  <si>
+    <t>Primitive data type</t>
+  </si>
+  <si>
+    <t>Object data type</t>
+  </si>
+  <si>
+    <t>p1.name="jane";</t>
+  </si>
+  <si>
+    <t>m.testing(p1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p.name="mike";</t>
+  </si>
+  <si>
+    <t>public void testing(Person p) {</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>main:225</t>
   </si>
 </sst>
 </file>
@@ -8163,7 +8265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="245">
+  <cellXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -8655,6 +8757,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8951,7 +9055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A53" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
@@ -37102,16 +37206,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N155"/>
+  <dimension ref="A2:N228"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G143" sqref="G143"/>
+    <sheetView tabSelected="1" topLeftCell="A208" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
@@ -38119,6 +38223,950 @@
       <c r="J155">
         <v>10</v>
       </c>
+    </row>
+    <row r="160" spans="2:14" ht="15.75" thickBot="1"/>
+    <row r="161" spans="2:12">
+      <c r="B161" s="33"/>
+      <c r="C161" s="34"/>
+      <c r="D161" s="34"/>
+      <c r="E161" s="34"/>
+      <c r="F161" s="34"/>
+      <c r="G161" s="34"/>
+      <c r="H161" s="34"/>
+      <c r="I161" s="34"/>
+      <c r="J161" s="34"/>
+      <c r="K161" s="34"/>
+      <c r="L161" s="35"/>
+    </row>
+    <row r="162" spans="2:12">
+      <c r="B162" s="36"/>
+      <c r="C162" s="30"/>
+      <c r="D162" s="30"/>
+      <c r="E162" s="30"/>
+      <c r="F162" s="30"/>
+      <c r="G162" s="30" t="s">
+        <v>2479</v>
+      </c>
+      <c r="H162" s="30"/>
+      <c r="I162" s="30"/>
+      <c r="J162" s="30"/>
+      <c r="K162" s="30"/>
+      <c r="L162" s="37"/>
+    </row>
+    <row r="163" spans="2:12">
+      <c r="B163" s="36"/>
+      <c r="C163" s="30"/>
+      <c r="D163" s="30"/>
+      <c r="E163" s="30"/>
+      <c r="F163" s="30"/>
+      <c r="G163" s="30"/>
+      <c r="H163" s="30"/>
+      <c r="I163" s="30"/>
+      <c r="J163" s="30"/>
+      <c r="K163" s="30"/>
+      <c r="L163" s="37"/>
+    </row>
+    <row r="164" spans="2:12">
+      <c r="B164" s="36" t="s">
+        <v>2477</v>
+      </c>
+      <c r="C164" s="30"/>
+      <c r="D164" s="30"/>
+      <c r="E164" s="30"/>
+      <c r="F164" s="30"/>
+      <c r="G164" s="46"/>
+      <c r="H164" s="30"/>
+      <c r="I164" s="30"/>
+      <c r="J164" s="30"/>
+      <c r="K164" s="30"/>
+      <c r="L164" s="37"/>
+    </row>
+    <row r="165" spans="2:12">
+      <c r="B165" s="36" t="s">
+        <v>2478</v>
+      </c>
+      <c r="C165" s="30"/>
+      <c r="D165" s="30"/>
+      <c r="E165" s="30"/>
+      <c r="F165" s="30"/>
+      <c r="G165" s="46" t="s">
+        <v>2482</v>
+      </c>
+      <c r="H165" s="30"/>
+      <c r="I165" s="30"/>
+      <c r="J165" s="30"/>
+      <c r="K165" s="30"/>
+      <c r="L165" s="37"/>
+    </row>
+    <row r="166" spans="2:12">
+      <c r="B166" s="36"/>
+      <c r="C166" s="30"/>
+      <c r="D166" s="30"/>
+      <c r="E166" s="30"/>
+      <c r="F166" s="30"/>
+      <c r="G166" s="46" t="s">
+        <v>2481</v>
+      </c>
+      <c r="H166" s="30"/>
+      <c r="I166" s="30"/>
+      <c r="J166" s="30"/>
+      <c r="K166" s="30"/>
+      <c r="L166" s="37"/>
+    </row>
+    <row r="167" spans="2:12">
+      <c r="B167" s="36"/>
+      <c r="C167" s="30"/>
+      <c r="D167" s="30"/>
+      <c r="E167" s="30"/>
+      <c r="F167" s="30"/>
+      <c r="G167" s="46" t="s">
+        <v>2480</v>
+      </c>
+      <c r="H167" s="30"/>
+      <c r="I167" s="30"/>
+      <c r="J167" s="30"/>
+      <c r="K167" s="30"/>
+      <c r="L167" s="37"/>
+    </row>
+    <row r="168" spans="2:12">
+      <c r="B168" s="36"/>
+      <c r="C168" s="30"/>
+      <c r="D168" s="30"/>
+      <c r="E168" s="30"/>
+      <c r="F168" s="30"/>
+      <c r="G168" s="46" t="s">
+        <v>2482</v>
+      </c>
+      <c r="H168" s="30"/>
+      <c r="I168" s="30"/>
+      <c r="J168" s="30"/>
+      <c r="K168" s="30"/>
+      <c r="L168" s="37"/>
+    </row>
+    <row r="169" spans="2:12">
+      <c r="B169" s="36"/>
+      <c r="C169" s="30"/>
+      <c r="D169" s="30"/>
+      <c r="E169" s="30"/>
+      <c r="F169" s="30"/>
+      <c r="G169" s="46" t="s">
+        <v>2481</v>
+      </c>
+      <c r="H169" s="30"/>
+      <c r="I169" s="30"/>
+      <c r="J169" s="30"/>
+      <c r="K169" s="30"/>
+      <c r="L169" s="37"/>
+    </row>
+    <row r="170" spans="2:12">
+      <c r="B170" s="36"/>
+      <c r="C170" s="30"/>
+      <c r="D170" s="30"/>
+      <c r="E170" s="30"/>
+      <c r="F170" s="30"/>
+      <c r="G170" s="46" t="s">
+        <v>2480</v>
+      </c>
+      <c r="H170" s="30"/>
+      <c r="I170" s="30"/>
+      <c r="J170" s="30"/>
+      <c r="K170" s="30"/>
+      <c r="L170" s="37"/>
+    </row>
+    <row r="171" spans="2:12">
+      <c r="B171" s="36"/>
+      <c r="C171" s="30"/>
+      <c r="D171" s="30"/>
+      <c r="E171" s="30"/>
+      <c r="F171" s="30"/>
+      <c r="G171" s="46" t="s">
+        <v>2482</v>
+      </c>
+      <c r="H171" s="30"/>
+      <c r="I171" s="30"/>
+      <c r="J171" s="30"/>
+      <c r="K171" s="30"/>
+      <c r="L171" s="37"/>
+    </row>
+    <row r="172" spans="2:12">
+      <c r="B172" s="36"/>
+      <c r="C172" s="30"/>
+      <c r="D172" s="30"/>
+      <c r="E172" s="30"/>
+      <c r="F172" s="30"/>
+      <c r="G172" s="46" t="s">
+        <v>2481</v>
+      </c>
+      <c r="H172" s="30"/>
+      <c r="I172" s="30"/>
+      <c r="J172" s="30"/>
+      <c r="K172" s="30"/>
+      <c r="L172" s="37"/>
+    </row>
+    <row r="173" spans="2:12">
+      <c r="B173" s="36"/>
+      <c r="C173" s="30"/>
+      <c r="D173" s="30"/>
+      <c r="E173" s="30"/>
+      <c r="F173" s="30"/>
+      <c r="G173" s="46" t="s">
+        <v>2480</v>
+      </c>
+      <c r="H173" s="30"/>
+      <c r="I173" s="30"/>
+      <c r="J173" s="30"/>
+      <c r="K173" s="30"/>
+      <c r="L173" s="37"/>
+    </row>
+    <row r="174" spans="2:12">
+      <c r="B174" s="36"/>
+      <c r="C174" s="30"/>
+      <c r="D174" s="30"/>
+      <c r="E174" s="30"/>
+      <c r="F174" s="30"/>
+      <c r="G174" s="46" t="s">
+        <v>2482</v>
+      </c>
+      <c r="H174" s="30"/>
+      <c r="I174" s="30"/>
+      <c r="J174" s="30"/>
+      <c r="K174" s="30"/>
+      <c r="L174" s="37"/>
+    </row>
+    <row r="175" spans="2:12">
+      <c r="B175" s="36"/>
+      <c r="C175" s="30"/>
+      <c r="D175" s="30"/>
+      <c r="E175" s="30"/>
+      <c r="F175" s="30"/>
+      <c r="G175" s="46" t="s">
+        <v>2481</v>
+      </c>
+      <c r="H175" s="30"/>
+      <c r="I175" s="30"/>
+      <c r="J175" s="30"/>
+      <c r="K175" s="30"/>
+      <c r="L175" s="37"/>
+    </row>
+    <row r="176" spans="2:12">
+      <c r="B176" s="36"/>
+      <c r="C176" s="30"/>
+      <c r="D176" s="30"/>
+      <c r="E176" s="30"/>
+      <c r="F176" s="30"/>
+      <c r="G176" s="46" t="s">
+        <v>2480</v>
+      </c>
+      <c r="H176" s="30"/>
+      <c r="I176" s="30"/>
+      <c r="J176" s="30"/>
+      <c r="K176" s="30"/>
+      <c r="L176" s="37"/>
+    </row>
+    <row r="177" spans="1:12">
+      <c r="B177" s="36"/>
+      <c r="C177" s="30"/>
+      <c r="D177" s="30"/>
+      <c r="E177" s="30"/>
+      <c r="F177" s="30"/>
+      <c r="G177" s="46" t="s">
+        <v>2476</v>
+      </c>
+      <c r="H177" s="30"/>
+      <c r="I177" s="30"/>
+      <c r="J177" s="30"/>
+      <c r="K177" s="30"/>
+      <c r="L177" s="37"/>
+    </row>
+    <row r="178" spans="1:12">
+      <c r="B178" s="36"/>
+      <c r="C178" s="30"/>
+      <c r="D178" s="30"/>
+      <c r="E178" s="30"/>
+      <c r="F178" s="30"/>
+      <c r="H178" s="30"/>
+      <c r="I178" s="30"/>
+      <c r="J178" s="30"/>
+      <c r="K178" s="30"/>
+      <c r="L178" s="37"/>
+    </row>
+    <row r="179" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B179" s="38"/>
+      <c r="C179" s="39"/>
+      <c r="D179" s="39"/>
+      <c r="E179" s="39"/>
+      <c r="F179" s="39"/>
+      <c r="G179" s="39"/>
+      <c r="H179" s="39"/>
+      <c r="I179" s="39"/>
+      <c r="J179" s="39"/>
+      <c r="K179" s="39"/>
+      <c r="L179" s="40"/>
+    </row>
+    <row r="186" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="187" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A187" t="s">
+        <v>2483</v>
+      </c>
+      <c r="D187" s="33"/>
+      <c r="E187" s="34"/>
+      <c r="F187" s="34"/>
+      <c r="G187" s="34"/>
+      <c r="H187" s="34"/>
+      <c r="I187" s="34"/>
+      <c r="J187" s="34"/>
+      <c r="K187" s="34"/>
+      <c r="L187" s="35"/>
+    </row>
+    <row r="188" spans="1:12">
+      <c r="B188" t="s">
+        <v>2484</v>
+      </c>
+      <c r="D188" s="36" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E188" s="30" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F188" s="30"/>
+      <c r="G188" s="30"/>
+      <c r="H188" s="30"/>
+      <c r="I188" s="30" t="s">
+        <v>431</v>
+      </c>
+      <c r="J188" s="33"/>
+      <c r="K188" s="35"/>
+      <c r="L188" s="37"/>
+    </row>
+    <row r="189" spans="1:12">
+      <c r="B189" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D189" s="53" t="s">
+        <v>2494</v>
+      </c>
+      <c r="E189" s="54" t="s">
+        <v>431</v>
+      </c>
+      <c r="F189" s="30"/>
+      <c r="G189" s="30"/>
+      <c r="H189" s="30"/>
+      <c r="I189" s="30"/>
+      <c r="J189" s="36"/>
+      <c r="K189" s="37"/>
+      <c r="L189" s="37"/>
+    </row>
+    <row r="190" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B190" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D190" s="53" t="s">
+        <v>554</v>
+      </c>
+      <c r="E190" s="54">
+        <v>10</v>
+      </c>
+      <c r="F190" s="30"/>
+      <c r="G190" s="30"/>
+      <c r="H190" s="30"/>
+      <c r="I190" s="30"/>
+      <c r="J190" s="38"/>
+      <c r="K190" s="40"/>
+      <c r="L190" s="37"/>
+    </row>
+    <row r="191" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B191" t="s">
+        <v>2487</v>
+      </c>
+      <c r="D191" s="53" t="s">
+        <v>1924</v>
+      </c>
+      <c r="E191" s="54" t="s">
+        <v>2023</v>
+      </c>
+      <c r="F191" s="30"/>
+      <c r="G191" s="30"/>
+      <c r="H191" s="30"/>
+      <c r="I191" s="30"/>
+      <c r="J191" s="30"/>
+      <c r="K191" s="30"/>
+      <c r="L191" s="37"/>
+    </row>
+    <row r="192" spans="1:12">
+      <c r="B192" s="60" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D192" s="53" t="s">
+        <v>420</v>
+      </c>
+      <c r="E192" s="54">
+        <v>20</v>
+      </c>
+      <c r="F192" s="30"/>
+      <c r="G192" s="30"/>
+      <c r="H192" s="30"/>
+      <c r="I192" s="30" t="s">
+        <v>2023</v>
+      </c>
+      <c r="J192" s="33"/>
+      <c r="K192" s="35"/>
+      <c r="L192" s="37"/>
+    </row>
+    <row r="193" spans="1:12">
+      <c r="A193" t="s">
+        <v>162</v>
+      </c>
+      <c r="D193" s="53" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E193" s="54" t="s">
+        <v>2023</v>
+      </c>
+      <c r="F193" s="30"/>
+      <c r="G193" s="30"/>
+      <c r="H193" s="30"/>
+      <c r="I193" s="30"/>
+      <c r="J193" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="K193" s="55" t="s">
+        <v>542</v>
+      </c>
+      <c r="L193" s="37"/>
+    </row>
+    <row r="194" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A194" t="s">
+        <v>1901</v>
+      </c>
+      <c r="D194" s="53"/>
+      <c r="E194" s="54"/>
+      <c r="F194" s="30"/>
+      <c r="G194" s="30"/>
+      <c r="H194" s="30"/>
+      <c r="I194" s="30"/>
+      <c r="J194" s="56" t="s">
+        <v>2456</v>
+      </c>
+      <c r="K194" s="58">
+        <v>20</v>
+      </c>
+      <c r="L194" s="37"/>
+    </row>
+    <row r="195" spans="1:12">
+      <c r="B195" t="s">
+        <v>374</v>
+      </c>
+      <c r="D195" s="53"/>
+      <c r="E195" s="54"/>
+      <c r="F195" s="30"/>
+      <c r="G195" s="30"/>
+      <c r="H195" s="30"/>
+      <c r="I195" s="30"/>
+      <c r="J195" s="30"/>
+      <c r="K195" s="30"/>
+      <c r="L195" s="37"/>
+    </row>
+    <row r="196" spans="1:12">
+      <c r="B196" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D196" s="53"/>
+      <c r="E196" s="54"/>
+      <c r="F196" s="30"/>
+      <c r="G196" s="30"/>
+      <c r="H196" s="30"/>
+      <c r="I196" s="30"/>
+      <c r="J196" s="30"/>
+      <c r="K196" s="30"/>
+      <c r="L196" s="37"/>
+    </row>
+    <row r="197" spans="1:12">
+      <c r="A197" t="s">
+        <v>162</v>
+      </c>
+      <c r="D197" s="53"/>
+      <c r="E197" s="54"/>
+      <c r="F197" s="30"/>
+      <c r="G197" s="30"/>
+      <c r="H197" s="30"/>
+      <c r="I197" s="30"/>
+      <c r="J197" s="30"/>
+      <c r="K197" s="30"/>
+      <c r="L197" s="37"/>
+    </row>
+    <row r="198" spans="1:12">
+      <c r="A198" t="s">
+        <v>2493</v>
+      </c>
+      <c r="D198" s="245" t="s">
+        <v>2495</v>
+      </c>
+      <c r="E198" s="54"/>
+      <c r="F198" s="246" t="s">
+        <v>2497</v>
+      </c>
+      <c r="G198" s="30"/>
+      <c r="H198" s="30"/>
+      <c r="I198" s="30"/>
+      <c r="J198" s="30"/>
+      <c r="K198" s="30"/>
+      <c r="L198" s="37"/>
+    </row>
+    <row r="199" spans="1:12">
+      <c r="B199" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D199" s="53" t="s">
+        <v>2496</v>
+      </c>
+      <c r="E199" s="30"/>
+      <c r="F199" s="30"/>
+      <c r="G199" s="30"/>
+      <c r="H199" s="246" t="s">
+        <v>552</v>
+      </c>
+      <c r="I199" s="30"/>
+      <c r="J199" s="30"/>
+      <c r="K199" s="30"/>
+      <c r="L199" s="37"/>
+    </row>
+    <row r="200" spans="1:12">
+      <c r="B200" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D200" s="53">
+        <v>10</v>
+      </c>
+      <c r="E200" s="30"/>
+      <c r="F200" s="30"/>
+      <c r="G200" s="30"/>
+      <c r="H200" s="30"/>
+      <c r="I200" s="30"/>
+      <c r="J200" s="30"/>
+      <c r="K200" s="30"/>
+      <c r="L200" s="37"/>
+    </row>
+    <row r="201" spans="1:12">
+      <c r="B201" t="s">
+        <v>382</v>
+      </c>
+      <c r="D201" s="53" t="s">
+        <v>577</v>
+      </c>
+      <c r="E201" s="30"/>
+      <c r="F201" s="30"/>
+      <c r="G201" s="30"/>
+      <c r="H201" s="30"/>
+      <c r="I201" s="30"/>
+      <c r="J201" s="30"/>
+      <c r="K201" s="30"/>
+      <c r="L201" s="37"/>
+    </row>
+    <row r="202" spans="1:12">
+      <c r="B202" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D202" s="53">
+        <v>10</v>
+      </c>
+      <c r="E202" s="30"/>
+      <c r="F202" s="30"/>
+      <c r="G202" s="30"/>
+      <c r="H202" s="30" t="s">
+        <v>2499</v>
+      </c>
+      <c r="I202" s="30"/>
+      <c r="J202" s="30" t="s">
+        <v>2502</v>
+      </c>
+      <c r="K202" s="30"/>
+      <c r="L202" s="37"/>
+    </row>
+    <row r="203" spans="1:12">
+      <c r="B203" t="s">
+        <v>1895</v>
+      </c>
+      <c r="D203" s="53" t="s">
+        <v>542</v>
+      </c>
+      <c r="E203" s="30"/>
+      <c r="F203" s="30"/>
+      <c r="G203" s="30"/>
+      <c r="H203" s="30" t="s">
+        <v>2500</v>
+      </c>
+      <c r="I203" s="30"/>
+      <c r="J203" s="30"/>
+      <c r="K203" s="30"/>
+      <c r="L203" s="37"/>
+    </row>
+    <row r="204" spans="1:12">
+      <c r="B204" t="s">
+        <v>2490</v>
+      </c>
+      <c r="D204" s="53"/>
+      <c r="E204" s="30"/>
+      <c r="F204" s="30" t="s">
+        <v>2498</v>
+      </c>
+      <c r="G204" s="30"/>
+      <c r="H204" s="30" t="s">
+        <v>2501</v>
+      </c>
+      <c r="I204" s="30"/>
+      <c r="J204" s="30" t="s">
+        <v>2503</v>
+      </c>
+      <c r="K204" s="30"/>
+      <c r="L204" s="37"/>
+    </row>
+    <row r="205" spans="1:12">
+      <c r="B205" t="s">
+        <v>2491</v>
+      </c>
+      <c r="D205" s="53"/>
+      <c r="E205" s="30"/>
+      <c r="F205" s="30"/>
+      <c r="G205" s="30"/>
+      <c r="H205" s="30"/>
+      <c r="I205" s="30"/>
+      <c r="J205" s="30"/>
+      <c r="K205" s="30"/>
+      <c r="L205" s="37"/>
+    </row>
+    <row r="206" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B206" t="s">
+        <v>2492</v>
+      </c>
+      <c r="D206" s="56"/>
+      <c r="E206" s="39"/>
+      <c r="F206" s="39"/>
+      <c r="G206" s="39"/>
+      <c r="H206" s="39"/>
+      <c r="I206" s="39"/>
+      <c r="J206" s="39"/>
+      <c r="K206" s="39"/>
+      <c r="L206" s="40"/>
+    </row>
+    <row r="208" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="209" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A209" t="s">
+        <v>2483</v>
+      </c>
+      <c r="D209" s="33"/>
+      <c r="E209" s="34"/>
+      <c r="F209" s="34"/>
+      <c r="G209" s="34"/>
+      <c r="H209" s="34"/>
+      <c r="I209" s="34"/>
+      <c r="J209" s="34"/>
+      <c r="K209" s="34"/>
+      <c r="L209" s="35"/>
+    </row>
+    <row r="210" spans="1:12">
+      <c r="B210" t="s">
+        <v>2507</v>
+      </c>
+      <c r="D210" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="E210" s="30" t="s">
+        <v>2508</v>
+      </c>
+      <c r="F210" s="30"/>
+      <c r="G210" s="30"/>
+      <c r="H210" s="30"/>
+      <c r="I210" s="30" t="s">
+        <v>431</v>
+      </c>
+      <c r="J210" s="33"/>
+      <c r="K210" s="35"/>
+      <c r="L210" s="37"/>
+    </row>
+    <row r="211" spans="1:12">
+      <c r="B211" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D211" s="53" t="s">
+        <v>2494</v>
+      </c>
+      <c r="E211" s="54" t="s">
+        <v>431</v>
+      </c>
+      <c r="F211" s="30"/>
+      <c r="G211" s="30"/>
+      <c r="H211" s="30"/>
+      <c r="I211" s="30"/>
+      <c r="J211" s="36"/>
+      <c r="K211" s="37"/>
+      <c r="L211" s="37"/>
+    </row>
+    <row r="212" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B212" t="s">
+        <v>162</v>
+      </c>
+      <c r="D212" s="53" t="s">
+        <v>1924</v>
+      </c>
+      <c r="E212" s="54" t="s">
+        <v>2023</v>
+      </c>
+      <c r="F212" s="30"/>
+      <c r="G212" s="30"/>
+      <c r="H212" s="30"/>
+      <c r="I212" s="30"/>
+      <c r="J212" s="38"/>
+      <c r="K212" s="40"/>
+      <c r="L212" s="37"/>
+    </row>
+    <row r="213" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A213" t="s">
+        <v>162</v>
+      </c>
+      <c r="D213" s="53" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E213" s="54" t="s">
+        <v>2023</v>
+      </c>
+      <c r="F213" s="30"/>
+      <c r="G213" s="30"/>
+      <c r="H213" s="30"/>
+      <c r="I213" s="30"/>
+      <c r="J213" s="30"/>
+      <c r="K213" s="30"/>
+      <c r="L213" s="37"/>
+    </row>
+    <row r="214" spans="1:12">
+      <c r="B214" s="60"/>
+      <c r="D214" s="53"/>
+      <c r="E214" s="54"/>
+      <c r="F214" s="30"/>
+      <c r="G214" s="30"/>
+      <c r="H214" s="30"/>
+      <c r="I214" s="30" t="s">
+        <v>2023</v>
+      </c>
+      <c r="J214" s="33"/>
+      <c r="K214" s="35"/>
+      <c r="L214" s="37"/>
+    </row>
+    <row r="215" spans="1:12">
+      <c r="A215" t="s">
+        <v>1901</v>
+      </c>
+      <c r="D215" s="53"/>
+      <c r="E215" s="54"/>
+      <c r="F215" s="30"/>
+      <c r="G215" s="30"/>
+      <c r="H215" s="30"/>
+      <c r="I215" s="30"/>
+      <c r="J215" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="K215" s="55" t="s">
+        <v>577</v>
+      </c>
+      <c r="L215" s="37"/>
+    </row>
+    <row r="216" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B216" t="s">
+        <v>374</v>
+      </c>
+      <c r="D216" s="53"/>
+      <c r="E216" s="54"/>
+      <c r="F216" s="30"/>
+      <c r="G216" s="30"/>
+      <c r="H216" s="30"/>
+      <c r="I216" s="30"/>
+      <c r="J216" s="56" t="s">
+        <v>2456</v>
+      </c>
+      <c r="K216" s="58">
+        <v>20</v>
+      </c>
+      <c r="L216" s="37"/>
+    </row>
+    <row r="217" spans="1:12">
+      <c r="B217" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D217" s="53"/>
+      <c r="E217" s="54"/>
+      <c r="F217" s="30"/>
+      <c r="G217" s="30"/>
+      <c r="H217" s="30"/>
+      <c r="I217" s="30"/>
+      <c r="J217" s="30"/>
+      <c r="K217" s="30"/>
+      <c r="L217" s="37"/>
+    </row>
+    <row r="218" spans="1:12">
+      <c r="A218" t="s">
+        <v>162</v>
+      </c>
+      <c r="D218" s="53"/>
+      <c r="E218" s="54"/>
+      <c r="F218" s="30"/>
+      <c r="G218" s="30"/>
+      <c r="H218" s="30"/>
+      <c r="I218" s="30"/>
+      <c r="J218" s="30"/>
+      <c r="K218" s="30"/>
+      <c r="L218" s="37"/>
+    </row>
+    <row r="219" spans="1:12">
+      <c r="D219" s="53"/>
+      <c r="E219" s="54"/>
+      <c r="F219" s="30"/>
+      <c r="G219" s="30"/>
+      <c r="H219" s="30"/>
+      <c r="I219" s="30"/>
+      <c r="J219" s="30"/>
+      <c r="K219" s="30"/>
+      <c r="L219" s="37"/>
+    </row>
+    <row r="220" spans="1:12">
+      <c r="A220" t="s">
+        <v>2493</v>
+      </c>
+      <c r="D220" s="245" t="s">
+        <v>2495</v>
+      </c>
+      <c r="E220" s="54"/>
+      <c r="F220" s="246" t="s">
+        <v>2497</v>
+      </c>
+      <c r="G220" s="30"/>
+      <c r="H220" s="30"/>
+      <c r="I220" s="30"/>
+      <c r="J220" s="30"/>
+      <c r="K220" s="30"/>
+      <c r="L220" s="37"/>
+    </row>
+    <row r="221" spans="1:12">
+      <c r="B221" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D221" s="53" t="s">
+        <v>430</v>
+      </c>
+      <c r="E221" s="30"/>
+      <c r="F221" s="30"/>
+      <c r="G221" s="30"/>
+      <c r="H221" s="246" t="s">
+        <v>552</v>
+      </c>
+      <c r="I221" s="30"/>
+      <c r="J221" s="30"/>
+      <c r="K221" s="30"/>
+      <c r="L221" s="37"/>
+    </row>
+    <row r="222" spans="1:12">
+      <c r="B222" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D222" s="53" t="s">
+        <v>577</v>
+      </c>
+      <c r="E222" s="30"/>
+      <c r="F222" s="30"/>
+      <c r="G222" s="30"/>
+      <c r="H222" s="30"/>
+      <c r="I222" s="30"/>
+      <c r="J222" s="30"/>
+      <c r="K222" s="30"/>
+      <c r="L222" s="37"/>
+    </row>
+    <row r="223" spans="1:12">
+      <c r="B223" t="s">
+        <v>2492</v>
+      </c>
+      <c r="D223" s="53"/>
+      <c r="E223" s="30"/>
+      <c r="F223" s="30"/>
+      <c r="G223" s="30"/>
+      <c r="H223" s="30"/>
+      <c r="I223" s="30"/>
+      <c r="J223" s="30"/>
+      <c r="K223" s="30"/>
+      <c r="L223" s="37"/>
+    </row>
+    <row r="224" spans="1:12">
+      <c r="B224" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D224" s="53"/>
+      <c r="E224" s="30"/>
+      <c r="F224" s="30" t="s">
+        <v>2509</v>
+      </c>
+      <c r="G224" s="30"/>
+      <c r="H224" s="30" t="s">
+        <v>2499</v>
+      </c>
+      <c r="I224" s="30"/>
+      <c r="J224" s="30" t="s">
+        <v>2502</v>
+      </c>
+      <c r="K224" s="30"/>
+      <c r="L224" s="37"/>
+    </row>
+    <row r="225" spans="2:12">
+      <c r="B225" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D225" s="53"/>
+      <c r="E225" s="30"/>
+      <c r="F225" s="30"/>
+      <c r="G225" s="30"/>
+      <c r="H225" s="30" t="s">
+        <v>2500</v>
+      </c>
+      <c r="I225" s="30"/>
+      <c r="J225" s="30"/>
+      <c r="K225" s="30"/>
+      <c r="L225" s="37"/>
+    </row>
+    <row r="226" spans="2:12">
+      <c r="B226" t="s">
+        <v>2492</v>
+      </c>
+      <c r="D226" s="53"/>
+      <c r="E226" s="30"/>
+      <c r="F226" s="30"/>
+      <c r="G226" s="30"/>
+      <c r="H226" s="30" t="s">
+        <v>2501</v>
+      </c>
+      <c r="I226" s="30"/>
+      <c r="J226" s="30" t="s">
+        <v>2503</v>
+      </c>
+      <c r="K226" s="30"/>
+      <c r="L226" s="37"/>
+    </row>
+    <row r="227" spans="2:12">
+      <c r="D227" s="53"/>
+      <c r="E227" s="30"/>
+      <c r="F227" s="30"/>
+      <c r="G227" s="30"/>
+      <c r="H227" s="30"/>
+      <c r="I227" s="30"/>
+      <c r="J227" s="30"/>
+      <c r="K227" s="30"/>
+      <c r="L227" s="37"/>
+    </row>
+    <row r="228" spans="2:12" ht="15.75" thickBot="1">
+      <c r="D228" s="56"/>
+      <c r="E228" s="39"/>
+      <c r="F228" s="39"/>
+      <c r="G228" s="39"/>
+      <c r="H228" s="39"/>
+      <c r="I228" s="39"/>
+      <c r="J228" s="39"/>
+      <c r="K228" s="39"/>
+      <c r="L228" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
move jee files to jee project
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="19" activeTab="19"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="references-latest" sheetId="28" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="2812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5077" uniqueCount="2822">
   <si>
     <t>USER</t>
   </si>
@@ -8660,6 +8660,36 @@
   </si>
   <si>
     <t>name=john</t>
+  </si>
+  <si>
+    <t>&lt;Restaurant&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/Restaurant&gt;</t>
+  </si>
+  <si>
+    <t>&lt;name&gt;john&lt;/name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;customer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/customer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;address&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/address&gt;</t>
+  </si>
+  <si>
+    <t>&lt;city&gt;</t>
+  </si>
+  <si>
+    <t>&lt;state&gt;</t>
   </si>
 </sst>
 </file>
@@ -9691,6 +9721,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9706,14 +9739,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -21376,13 +21406,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1">
-      <c r="H3" s="256" t="s">
+      <c r="H3" s="257" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="257"/>
-      <c r="J3" s="257"/>
-      <c r="K3" s="257"/>
-      <c r="L3" s="258"/>
+      <c r="I3" s="258"/>
+      <c r="J3" s="258"/>
+      <c r="K3" s="258"/>
+      <c r="L3" s="259"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1">
       <c r="P4" t="s">
@@ -21419,20 +21449,20 @@
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1">
       <c r="F6" s="4"/>
-      <c r="G6" s="259" t="s">
+      <c r="G6" s="260" t="s">
         <v>1678</v>
       </c>
-      <c r="H6" s="260"/>
+      <c r="H6" s="261"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="259" t="s">
+      <c r="J6" s="260" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="260"/>
+      <c r="K6" s="261"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="259" t="s">
+      <c r="M6" s="260" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="260"/>
+      <c r="N6" s="261"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1">
       <c r="D7" s="128" t="s">
@@ -21456,20 +21486,20 @@
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1">
       <c r="F8" s="4"/>
-      <c r="G8" s="259" t="s">
+      <c r="G8" s="260" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="260"/>
+      <c r="H8" s="261"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="259" t="s">
+      <c r="J8" s="260" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="260"/>
+      <c r="K8" s="261"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="259" t="s">
+      <c r="M8" s="260" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="260"/>
+      <c r="N8" s="261"/>
       <c r="P8" t="s">
         <v>1684</v>
       </c>
@@ -22585,7 +22615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A222" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M239" sqref="M239"/>
     </sheetView>
   </sheetViews>
@@ -25561,7 +25591,7 @@
       <c r="N235" s="52">
         <v>10</v>
       </c>
-      <c r="O235" s="263" t="s">
+      <c r="O235" s="262" t="s">
         <v>2811</v>
       </c>
       <c r="P235" s="54"/>
@@ -25586,7 +25616,7 @@
       <c r="L236" s="54"/>
       <c r="M236" s="56"/>
       <c r="N236" s="58"/>
-      <c r="O236" s="263"/>
+      <c r="O236" s="262"/>
       <c r="P236" s="54"/>
       <c r="Q236" s="55"/>
     </row>
@@ -25609,7 +25639,7 @@
       <c r="L237" s="54"/>
       <c r="M237" s="54"/>
       <c r="N237" s="54"/>
-      <c r="O237" s="263"/>
+      <c r="O237" s="262"/>
       <c r="P237" s="54"/>
       <c r="Q237" s="55"/>
     </row>
@@ -25632,7 +25662,7 @@
       <c r="N238" s="52">
         <v>10</v>
       </c>
-      <c r="O238" s="263"/>
+      <c r="O238" s="262"/>
       <c r="P238" s="54"/>
       <c r="Q238" s="55"/>
     </row>
@@ -25649,7 +25679,7 @@
       <c r="L239" s="54"/>
       <c r="M239" s="56"/>
       <c r="N239" s="58"/>
-      <c r="O239" s="263"/>
+      <c r="O239" s="262"/>
       <c r="P239" s="54"/>
       <c r="Q239" s="55"/>
     </row>
@@ -25668,7 +25698,7 @@
       <c r="L240" s="54"/>
       <c r="M240" s="54"/>
       <c r="N240" s="54"/>
-      <c r="O240" s="263"/>
+      <c r="O240" s="262"/>
       <c r="P240" s="54"/>
       <c r="Q240" s="55"/>
     </row>
@@ -25693,7 +25723,7 @@
       <c r="N241" s="52">
         <v>10</v>
       </c>
-      <c r="O241" s="263"/>
+      <c r="O241" s="262"/>
       <c r="P241" s="54"/>
       <c r="Q241" s="55"/>
     </row>
@@ -25712,7 +25742,7 @@
       <c r="L242" s="54"/>
       <c r="M242" s="56"/>
       <c r="N242" s="58"/>
-      <c r="O242" s="263"/>
+      <c r="O242" s="262"/>
       <c r="P242" s="54"/>
       <c r="Q242" s="55"/>
     </row>
@@ -25729,7 +25759,7 @@
       <c r="L243" s="54"/>
       <c r="M243" s="54"/>
       <c r="N243" s="54"/>
-      <c r="O243" s="262"/>
+      <c r="O243" s="256"/>
       <c r="P243" s="54"/>
       <c r="Q243" s="55"/>
     </row>
@@ -38903,11 +38933,11 @@
       <c r="L6" s="46" t="s">
         <v>1615</v>
       </c>
-      <c r="M6" s="261" t="s">
+      <c r="M6" s="263" t="s">
         <v>1616</v>
       </c>
-      <c r="N6" s="261"/>
-      <c r="O6" s="261"/>
+      <c r="N6" s="263"/>
+      <c r="O6" s="263"/>
       <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
       <c r="R6" s="30"/>
@@ -41117,8 +41147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:M28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41474,6 +41504,9 @@
     </row>
     <row r="29" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>2812</v>
+      </c>
       <c r="G30" s="33" t="s">
         <v>2408</v>
       </c>
@@ -41486,6 +41519,9 @@
       <c r="M30" s="35"/>
     </row>
     <row r="31" spans="1:16">
+      <c r="B31" t="s">
+        <v>2814</v>
+      </c>
       <c r="G31" s="36"/>
       <c r="H31" s="30" t="s">
         <v>198</v>
@@ -41508,6 +41544,9 @@
       </c>
     </row>
     <row r="32" spans="1:16">
+      <c r="B32" t="s">
+        <v>2815</v>
+      </c>
       <c r="G32" s="36"/>
       <c r="H32" s="30" t="s">
         <v>203</v>
@@ -41529,7 +41568,10 @@
         <v>44553</v>
       </c>
     </row>
-    <row r="33" spans="3:15">
+    <row r="33" spans="1:15">
+      <c r="C33" t="s">
+        <v>2817</v>
+      </c>
       <c r="G33" s="36"/>
       <c r="H33" s="30" t="s">
         <v>198</v>
@@ -41551,7 +41593,10 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="34" spans="3:15">
+    <row r="34" spans="1:15">
+      <c r="C34" t="s">
+        <v>2818</v>
+      </c>
       <c r="G34" s="36"/>
       <c r="H34" s="41" t="s">
         <v>2402</v>
@@ -41570,7 +41615,10 @@
         <v>430</v>
       </c>
     </row>
-    <row r="35" spans="3:15" ht="15.75" thickBot="1">
+    <row r="35" spans="1:15" ht="15.75" thickBot="1">
+      <c r="D35" t="s">
+        <v>2820</v>
+      </c>
       <c r="G35" s="38"/>
       <c r="H35" s="39"/>
       <c r="I35" s="40"/>
@@ -41585,8 +41633,29 @@
         <v>850</v>
       </c>
     </row>
-    <row r="42" spans="3:15" ht="15.75" thickBot="1"/>
-    <row r="43" spans="3:15">
+    <row r="36" spans="1:15">
+      <c r="D36" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="C37" t="s">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="B38" t="s">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" t="s">
+        <v>2813</v>
+      </c>
+      <c r="C39" s="43"/>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="43" spans="1:15">
       <c r="G43" s="33"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -41596,7 +41665,7 @@
       <c r="N43" s="30"/>
       <c r="O43" s="37"/>
     </row>
-    <row r="44" spans="3:15" ht="15.75" thickBot="1">
+    <row r="44" spans="1:15" ht="15.75" thickBot="1">
       <c r="G44" s="36"/>
       <c r="H44" s="30"/>
       <c r="I44" s="30"/>
@@ -41606,20 +41675,19 @@
       <c r="N44" s="39"/>
       <c r="O44" s="40"/>
     </row>
-    <row r="45" spans="3:15">
-      <c r="C45" s="43"/>
+    <row r="45" spans="1:15">
       <c r="G45" s="36"/>
       <c r="H45" s="30"/>
       <c r="I45" s="30"/>
       <c r="J45" s="37"/>
     </row>
-    <row r="46" spans="3:15">
+    <row r="46" spans="1:15">
       <c r="G46" s="36"/>
       <c r="H46" s="30"/>
       <c r="I46" s="30"/>
       <c r="J46" s="37"/>
     </row>
-    <row r="47" spans="3:15" ht="15.75" thickBot="1">
+    <row r="47" spans="1:15" ht="15.75" thickBot="1">
       <c r="G47" s="38"/>
       <c r="H47" s="39"/>
       <c r="I47" s="39"/>

</xml_diff>